<commit_message>
added more js stuff
</commit_message>
<xml_diff>
--- a/business Stats/Book2.xlsx
+++ b/business Stats/Book2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Ujwal\git\business Stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F6A920-7FF2-4E38-9162-C0AC25AAC62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D9730C-AB88-40D9-8FE4-839B7B576E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{84D76DE3-8557-4722-B5C1-4893E077E0C2}"/>
   </bookViews>
@@ -955,27 +955,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -999,6 +978,27 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3950,7 +3950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AC71F3-EDAC-4C28-A1D6-182EE705764F}">
   <dimension ref="A1:P205"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A184" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="10" zoomScaleNormal="85" zoomScalePageLayoutView="10" workbookViewId="0">
       <selection activeCell="I205" sqref="I205"/>
     </sheetView>
   </sheetViews>
@@ -4029,45 +4029,45 @@
       <c r="A6" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="49" t="s">
+      <c r="K6" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="49"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
     </row>
     <row r="7" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="41">
         <v>1</v>
       </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="K7" s="49" t="s">
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="K7" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="49"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="57"/>
     </row>
     <row r="8" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
-      <c r="K8" s="49" t="s">
+      <c r="K8" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="49"/>
+      <c r="L8" s="57"/>
+      <c r="M8" s="57"/>
+      <c r="N8" s="57"/>
     </row>
     <row r="9" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="49" t="s">
+      <c r="K9" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="L9" s="49"/>
-      <c r="M9" s="49"/>
-      <c r="N9" s="49"/>
+      <c r="L9" s="57"/>
+      <c r="M9" s="57"/>
+      <c r="N9" s="57"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="37"/>
@@ -4076,48 +4076,48 @@
       <c r="A11" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="45" t="s">
+      <c r="K11" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="L11" s="44"/>
-      <c r="M11" s="44"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="53"/>
     </row>
     <row r="12" spans="1:14" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A12" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="K12" s="49" t="s">
+      <c r="K12" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="L12" s="49"/>
-      <c r="M12" s="49"/>
-      <c r="N12" s="49"/>
+      <c r="L12" s="57"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="57"/>
     </row>
     <row r="13" spans="1:14" ht="21.75" x14ac:dyDescent="0.25">
       <c r="A13" s="40"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="49"/>
-      <c r="M13" s="49"/>
-      <c r="N13" s="49"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="57"/>
     </row>
     <row r="14" spans="1:14" ht="21.75" x14ac:dyDescent="0.25">
       <c r="A14" s="40"/>
-      <c r="K14" s="49" t="s">
+      <c r="K14" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="L14" s="50"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="50"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="58"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="50"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="50"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="58"/>
+      <c r="M15" s="58"/>
+      <c r="N15" s="58"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
@@ -4125,10 +4125,10 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="K16" s="44"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="49"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="57"/>
+      <c r="N16" s="57"/>
     </row>
     <row r="17" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -4139,10 +4139,10 @@
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="49"/>
-      <c r="N17" s="49"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="57"/>
+      <c r="M17" s="57"/>
+      <c r="N17" s="57"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
@@ -4386,10 +4386,10 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="46" t="s">
+      <c r="B34" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="46"/>
+      <c r="C34" s="55"/>
       <c r="F34" s="11"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -4514,17 +4514,17 @@
       <c r="A48" s="41">
         <v>1</v>
       </c>
-      <c r="B48" s="47"/>
-      <c r="C48" s="47"/>
-      <c r="K48" s="48">
+      <c r="B48" s="56"/>
+      <c r="C48" s="56"/>
+      <c r="K48" s="59">
         <v>1</v>
       </c>
-      <c r="L48" s="48"/>
+      <c r="L48" s="59"/>
     </row>
     <row r="49" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="36"/>
-      <c r="K49" s="48"/>
-      <c r="L49" s="48"/>
+      <c r="K49" s="59"/>
+      <c r="L49" s="59"/>
     </row>
     <row r="50" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="36" t="s">
@@ -4847,10 +4847,10 @@
       <c r="C72" s="11"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B75" s="46" t="s">
+      <c r="B75" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="C75" s="46"/>
+      <c r="C75" s="55"/>
       <c r="F75" s="11"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
@@ -4900,20 +4900,20 @@
       </c>
     </row>
     <row r="88" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="K88" s="44" t="s">
+      <c r="K88" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="L88" s="44"/>
-      <c r="M88" s="44"/>
-      <c r="N88" s="44"/>
-      <c r="O88" s="44"/>
+      <c r="L88" s="53"/>
+      <c r="M88" s="53"/>
+      <c r="N88" s="53"/>
+      <c r="O88" s="53"/>
     </row>
     <row r="89" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="K89" s="44"/>
-      <c r="L89" s="44"/>
-      <c r="M89" s="44"/>
-      <c r="N89" s="44"/>
-      <c r="O89" s="44"/>
+      <c r="K89" s="53"/>
+      <c r="L89" s="53"/>
+      <c r="M89" s="53"/>
+      <c r="N89" s="53"/>
+      <c r="O89" s="53"/>
     </row>
     <row r="90" spans="2:16" x14ac:dyDescent="0.25">
       <c r="K90" t="s">
@@ -4936,7 +4936,7 @@
       </c>
     </row>
     <row r="91" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B91" s="51" t="s">
+      <c r="B91" s="44" t="s">
         <v>1</v>
       </c>
       <c r="K91" t="s">
@@ -4967,14 +4967,14 @@
       <c r="B93">
         <v>7</v>
       </c>
-      <c r="K93" s="44" t="s">
+      <c r="K93" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="L93" s="44"/>
-      <c r="M93" s="44"/>
-      <c r="N93" s="44"/>
-      <c r="O93" s="44"/>
-      <c r="P93" s="44"/>
+      <c r="L93" s="53"/>
+      <c r="M93" s="53"/>
+      <c r="N93" s="53"/>
+      <c r="O93" s="53"/>
+      <c r="P93" s="53"/>
     </row>
     <row r="94" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B94">
@@ -4990,25 +4990,25 @@
       <c r="B96">
         <v>5</v>
       </c>
-      <c r="J96" s="45" t="s">
+      <c r="J96" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="K96" s="44"/>
-      <c r="N96" s="45" t="s">
+      <c r="K96" s="53"/>
+      <c r="N96" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="O96" s="45"/>
+      <c r="O96" s="54"/>
     </row>
     <row r="97" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>4</v>
       </c>
-      <c r="J97" s="44" t="s">
+      <c r="J97" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="K97" s="44"/>
-      <c r="L97" s="44"/>
-      <c r="M97" s="44"/>
+      <c r="K97" s="53"/>
+      <c r="L97" s="53"/>
+      <c r="M97" s="53"/>
       <c r="N97" t="s">
         <v>1</v>
       </c>
@@ -5020,12 +5020,12 @@
       <c r="B98">
         <v>10</v>
       </c>
-      <c r="J98" s="44" t="s">
+      <c r="J98" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="K98" s="44"/>
-      <c r="L98" s="44"/>
-      <c r="M98" s="44"/>
+      <c r="K98" s="53"/>
+      <c r="L98" s="53"/>
+      <c r="M98" s="53"/>
       <c r="N98">
         <v>2</v>
       </c>
@@ -5037,12 +5037,12 @@
       <c r="B99">
         <v>6</v>
       </c>
-      <c r="J99" s="44" t="s">
+      <c r="J99" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="K99" s="44"/>
-      <c r="L99" s="44"/>
-      <c r="M99" s="44"/>
+      <c r="K99" s="53"/>
+      <c r="L99" s="53"/>
+      <c r="M99" s="53"/>
       <c r="N99">
         <v>7</v>
       </c>
@@ -5078,14 +5078,14 @@
       </c>
     </row>
     <row r="104" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="N104" s="44" t="s">
+      <c r="N104" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="O104" s="44"/>
+      <c r="O104" s="53"/>
     </row>
     <row r="105" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="N105" s="44"/>
-      <c r="O105" s="44"/>
+      <c r="N105" s="53"/>
+      <c r="O105" s="53"/>
     </row>
     <row r="106" spans="2:15" x14ac:dyDescent="0.25">
       <c r="N106" t="s">
@@ -5133,31 +5133,31 @@
       </c>
     </row>
     <row r="122" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K122" s="45" t="s">
+      <c r="K122" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="L122" s="44"/>
+      <c r="L122" s="53"/>
     </row>
     <row r="123" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K123" s="44" t="s">
+      <c r="K123" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="L123" s="44"/>
+      <c r="L123" s="53"/>
       <c r="M123" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="135" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="44" t="s">
+      <c r="A135" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B135" s="44"/>
-      <c r="C135" s="44"/>
-      <c r="D135" s="44"/>
-      <c r="E135" s="44"/>
-      <c r="F135" s="44"/>
-      <c r="G135" s="44"/>
-      <c r="H135" s="44"/>
+      <c r="B135" s="53"/>
+      <c r="C135" s="53"/>
+      <c r="D135" s="53"/>
+      <c r="E135" s="53"/>
+      <c r="F135" s="53"/>
+      <c r="G135" s="53"/>
+      <c r="H135" s="53"/>
       <c r="J135" t="s">
         <v>64</v>
       </c>
@@ -5171,22 +5171,22 @@
       <c r="F136" s="3"/>
       <c r="G136" s="3"/>
       <c r="H136" s="3"/>
-      <c r="J136" s="52" t="s">
+      <c r="J136" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="K136" s="53" t="s">
+      <c r="K136" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="L136" s="54" t="s">
+      <c r="L136" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="M136" s="53" t="s">
+      <c r="M136" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="N136" s="53" t="s">
+      <c r="N136" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="O136" s="53" t="s">
+      <c r="O136" s="46" t="s">
         <v>69</v>
       </c>
     </row>
@@ -5209,22 +5209,22 @@
       <c r="F137">
         <v>4</v>
       </c>
-      <c r="J137" s="55" t="s">
+      <c r="J137" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="K137" s="56">
+      <c r="K137" s="49">
         <v>2</v>
       </c>
-      <c r="L137" s="56">
+      <c r="L137" s="49">
         <v>10</v>
       </c>
-      <c r="M137" s="56">
+      <c r="M137" s="49">
         <v>16</v>
       </c>
-      <c r="N137" s="56">
+      <c r="N137" s="49">
         <v>10</v>
       </c>
-      <c r="O137" s="56">
+      <c r="O137" s="49">
         <v>4</v>
       </c>
     </row>
@@ -5565,16 +5565,16 @@
       </c>
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A153" s="44" t="s">
+      <c r="A153" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B153" s="44"/>
-      <c r="C153" s="44"/>
-      <c r="D153" s="44"/>
-      <c r="E153" s="44"/>
-      <c r="F153" s="44"/>
-      <c r="G153" s="44"/>
-      <c r="H153" s="44"/>
+      <c r="B153" s="53"/>
+      <c r="C153" s="53"/>
+      <c r="D153" s="53"/>
+      <c r="E153" s="53"/>
+      <c r="F153" s="53"/>
+      <c r="G153" s="53"/>
+      <c r="H153" s="53"/>
       <c r="I153" t="s">
         <v>82</v>
       </c>
@@ -5587,7 +5587,7 @@
       <c r="I154" t="s">
         <v>83</v>
       </c>
-      <c r="J154" s="51" t="str">
+      <c r="J154" s="44" t="str">
         <f>M136</f>
         <v>20-30</v>
       </c>
@@ -5620,20 +5620,20 @@
       </c>
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J160" s="45" t="s">
+      <c r="J160" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="K160" s="44"/>
+      <c r="K160" s="53"/>
     </row>
     <row r="161" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J161" s="44" t="s">
+      <c r="J161" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="K161" s="44"/>
-      <c r="L161" s="44"/>
-      <c r="M161" s="44"/>
-      <c r="N161" s="44"/>
-      <c r="O161" s="44"/>
+      <c r="K161" s="53"/>
+      <c r="L161" s="53"/>
+      <c r="M161" s="53"/>
+      <c r="N161" s="53"/>
+      <c r="O161" s="53"/>
     </row>
     <row r="162" spans="10:15" x14ac:dyDescent="0.25">
       <c r="J162" t="s">
@@ -5663,15 +5663,15 @@
       </c>
     </row>
     <row r="185" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J185" s="44" t="s">
+      <c r="J185" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="K185" s="44"/>
-      <c r="L185" s="44"/>
-      <c r="M185" s="44"/>
-      <c r="N185" s="44"/>
-      <c r="O185" s="44"/>
-      <c r="P185" s="44"/>
+      <c r="K185" s="53"/>
+      <c r="L185" s="53"/>
+      <c r="M185" s="53"/>
+      <c r="N185" s="53"/>
+      <c r="O185" s="53"/>
+      <c r="P185" s="53"/>
     </row>
     <row r="186" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="42" t="s">
@@ -5683,46 +5683,46 @@
       <c r="A187" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="K187" s="52" t="s">
+      <c r="K187" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="L187" s="53">
+      <c r="L187" s="46">
         <v>10</v>
       </c>
-      <c r="M187" s="53">
+      <c r="M187" s="46">
         <v>20</v>
       </c>
-      <c r="N187" s="53">
+      <c r="N187" s="46">
         <v>30</v>
       </c>
-      <c r="O187" s="53">
+      <c r="O187" s="46">
         <v>40</v>
       </c>
-      <c r="P187" s="59"/>
+      <c r="P187" s="52"/>
     </row>
     <row r="188" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K188" s="55" t="s">
+      <c r="K188" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="L188" s="56">
+      <c r="L188" s="49">
         <v>2</v>
       </c>
-      <c r="M188" s="56">
+      <c r="M188" s="49">
         <v>5</v>
       </c>
-      <c r="N188" s="56">
+      <c r="N188" s="49">
         <v>3</v>
       </c>
-      <c r="O188" s="56">
+      <c r="O188" s="49">
         <v>2</v>
       </c>
-      <c r="P188" s="59"/>
+      <c r="P188" s="52"/>
     </row>
     <row r="189" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K189" s="43"/>
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A190" s="57" t="s">
+      <c r="A190" s="50" t="s">
         <v>1</v>
       </c>
       <c r="I190" t="s">
@@ -5799,7 +5799,7 @@
       <c r="A200" t="s">
         <v>40</v>
       </c>
-      <c r="B200" s="58">
+      <c r="B200" s="51">
         <f>_xlfn.STDEV.P(A190:A197)</f>
         <v>2.2314999074019015</v>
       </c>
@@ -5828,21 +5828,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A135:H135"/>
-    <mergeCell ref="A153:H153"/>
-    <mergeCell ref="J160:K160"/>
-    <mergeCell ref="J161:O161"/>
-    <mergeCell ref="J185:P185"/>
-    <mergeCell ref="J99:M99"/>
-    <mergeCell ref="N96:O96"/>
-    <mergeCell ref="N104:O105"/>
-    <mergeCell ref="K122:L122"/>
-    <mergeCell ref="K123:L123"/>
-    <mergeCell ref="K88:O89"/>
-    <mergeCell ref="K93:P93"/>
-    <mergeCell ref="J96:K96"/>
-    <mergeCell ref="J97:M97"/>
-    <mergeCell ref="J98:M98"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="B7:C7"/>
@@ -5858,6 +5843,21 @@
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="L14:N15"/>
     <mergeCell ref="K48:L49"/>
+    <mergeCell ref="K88:O89"/>
+    <mergeCell ref="K93:P93"/>
+    <mergeCell ref="J96:K96"/>
+    <mergeCell ref="J97:M97"/>
+    <mergeCell ref="J98:M98"/>
+    <mergeCell ref="J99:M99"/>
+    <mergeCell ref="N96:O96"/>
+    <mergeCell ref="N104:O105"/>
+    <mergeCell ref="K122:L122"/>
+    <mergeCell ref="K123:L123"/>
+    <mergeCell ref="A135:H135"/>
+    <mergeCell ref="A153:H153"/>
+    <mergeCell ref="J160:K160"/>
+    <mergeCell ref="J161:O161"/>
+    <mergeCell ref="J185:P185"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added more excel content
</commit_message>
<xml_diff>
--- a/business Stats/Book2.xlsx
+++ b/business Stats/Book2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Ujwal\git\business Stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BE90F0-2146-487A-9331-D1D268CF78EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2D5C72-BBB8-4451-A81F-9B6B0C87880C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{84D76DE3-8557-4722-B5C1-4893E077E0C2}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="162">
   <si>
     <t>Calculate the correlation of the following data</t>
   </si>
@@ -664,13 +664,80 @@
   <si>
     <t>F</t>
   </si>
+  <si>
+    <t xml:space="preserve">From the following find the Mean and SD </t>
+  </si>
+  <si>
+    <t>10--15</t>
+  </si>
+  <si>
+    <t>15-20</t>
+  </si>
+  <si>
+    <t>20-25</t>
+  </si>
+  <si>
+    <t>25-30</t>
+  </si>
+  <si>
+    <t>30-35</t>
+  </si>
+  <si>
+    <t>fx^2</t>
+  </si>
+  <si>
+    <t>Totals</t>
+  </si>
+  <si>
+    <t>A random sample of 50 gave a mean of 75 kg and SD of 1.5kg</t>
+  </si>
+  <si>
+    <t>Find the 95% confidence limit of the population mean</t>
+  </si>
+  <si>
+    <t>critical value</t>
+  </si>
+  <si>
+    <t>probablity</t>
+  </si>
+  <si>
+    <t>μ</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>μ(low)</t>
+  </si>
+  <si>
+    <t>μ(upp)</t>
+  </si>
+  <si>
+    <t>α</t>
+  </si>
+  <si>
+    <t>σ</t>
+  </si>
+  <si>
+    <t>A random sample of 100 students is found to have mean weight of 55 kg and</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and SD of 5kg test hypothesis that the mean test hypothesis that the mean weight </t>
+  </si>
+  <si>
+    <t>of the pop-n is 52 kg at 5% level of significance</t>
+  </si>
+  <si>
+    <t>s mean</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1104,7 +1171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1223,11 +1290,26 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1235,21 +1317,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5187,10 +5255,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AC71F3-EDAC-4C28-A1D6-182EE705764F}">
-  <dimension ref="A1:P365"/>
+  <dimension ref="A1:P400"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A349" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A363" sqref="A363"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A382" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J404" sqref="J404"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5269,45 +5337,45 @@
       <c r="A6" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="58" t="s">
+      <c r="K6" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="63"/>
     </row>
     <row r="7" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="41">
         <v>1</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="K7" s="58" t="s">
+      <c r="B7" s="66"/>
+      <c r="C7" s="66"/>
+      <c r="K7" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="L7" s="58"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63"/>
+      <c r="N7" s="63"/>
     </row>
     <row r="8" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
-      <c r="K8" s="58" t="s">
+      <c r="K8" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="L8" s="58"/>
-      <c r="M8" s="58"/>
-      <c r="N8" s="58"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="63"/>
+      <c r="N8" s="63"/>
     </row>
     <row r="9" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="58" t="s">
+      <c r="K9" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="L9" s="58"/>
-      <c r="M9" s="58"/>
-      <c r="N9" s="58"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="63"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="37"/>
@@ -5316,48 +5384,48 @@
       <c r="A11" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="54" t="s">
+      <c r="K11" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="L11" s="55"/>
-      <c r="M11" s="55"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="60"/>
     </row>
     <row r="12" spans="1:14" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A12" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="K12" s="58" t="s">
+      <c r="K12" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="L12" s="58"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="58"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
     </row>
     <row r="13" spans="1:14" ht="21.75" x14ac:dyDescent="0.25">
       <c r="A13" s="40"/>
-      <c r="K13" s="58"/>
-      <c r="L13" s="58"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="58"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="63"/>
     </row>
     <row r="14" spans="1:14" ht="21.75" x14ac:dyDescent="0.25">
       <c r="A14" s="40"/>
-      <c r="K14" s="58" t="s">
+      <c r="K14" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="L14" s="59"/>
-      <c r="M14" s="59"/>
-      <c r="N14" s="59"/>
+      <c r="L14" s="64"/>
+      <c r="M14" s="64"/>
+      <c r="N14" s="64"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
-      <c r="K15" s="58"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="59"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="64"/>
+      <c r="N15" s="64"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
@@ -5365,10 +5433,10 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="K16" s="55"/>
-      <c r="L16" s="58"/>
-      <c r="M16" s="58"/>
-      <c r="N16" s="58"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="63"/>
+      <c r="M16" s="63"/>
+      <c r="N16" s="63"/>
     </row>
     <row r="17" spans="1:14" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -5379,10 +5447,10 @@
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-      <c r="K17" s="55"/>
-      <c r="L17" s="58"/>
-      <c r="M17" s="58"/>
-      <c r="N17" s="58"/>
+      <c r="K17" s="60"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="63"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
@@ -5626,10 +5694,10 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="56" t="s">
+      <c r="B34" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="56"/>
+      <c r="C34" s="65"/>
       <c r="F34" s="11"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -5754,17 +5822,17 @@
       <c r="A48" s="41">
         <v>1</v>
       </c>
-      <c r="B48" s="57"/>
-      <c r="C48" s="57"/>
-      <c r="K48" s="60">
+      <c r="B48" s="66"/>
+      <c r="C48" s="66"/>
+      <c r="K48" s="62">
         <v>1</v>
       </c>
-      <c r="L48" s="60"/>
+      <c r="L48" s="62"/>
     </row>
     <row r="49" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="36"/>
-      <c r="K49" s="60"/>
-      <c r="L49" s="60"/>
+      <c r="K49" s="62"/>
+      <c r="L49" s="62"/>
     </row>
     <row r="50" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="36" t="s">
@@ -6087,10 +6155,10 @@
       <c r="C72" s="11"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B75" s="56" t="s">
+      <c r="B75" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="C75" s="56"/>
+      <c r="C75" s="65"/>
       <c r="F75" s="11"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
@@ -6140,20 +6208,20 @@
       </c>
     </row>
     <row r="88" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="K88" s="55" t="s">
+      <c r="K88" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="L88" s="55"/>
-      <c r="M88" s="55"/>
-      <c r="N88" s="55"/>
-      <c r="O88" s="55"/>
+      <c r="L88" s="60"/>
+      <c r="M88" s="60"/>
+      <c r="N88" s="60"/>
+      <c r="O88" s="60"/>
     </row>
     <row r="89" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="K89" s="55"/>
-      <c r="L89" s="55"/>
-      <c r="M89" s="55"/>
-      <c r="N89" s="55"/>
-      <c r="O89" s="55"/>
+      <c r="K89" s="60"/>
+      <c r="L89" s="60"/>
+      <c r="M89" s="60"/>
+      <c r="N89" s="60"/>
+      <c r="O89" s="60"/>
     </row>
     <row r="90" spans="2:16" x14ac:dyDescent="0.25">
       <c r="K90" t="s">
@@ -6207,14 +6275,14 @@
       <c r="B93">
         <v>7</v>
       </c>
-      <c r="K93" s="55" t="s">
+      <c r="K93" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="L93" s="55"/>
-      <c r="M93" s="55"/>
-      <c r="N93" s="55"/>
-      <c r="O93" s="55"/>
-      <c r="P93" s="55"/>
+      <c r="L93" s="60"/>
+      <c r="M93" s="60"/>
+      <c r="N93" s="60"/>
+      <c r="O93" s="60"/>
+      <c r="P93" s="60"/>
     </row>
     <row r="94" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B94">
@@ -6230,25 +6298,25 @@
       <c r="B96">
         <v>5</v>
       </c>
-      <c r="J96" s="54" t="s">
+      <c r="J96" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="K96" s="55"/>
-      <c r="N96" s="54" t="s">
+      <c r="K96" s="60"/>
+      <c r="N96" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="O96" s="54"/>
+      <c r="O96" s="61"/>
     </row>
     <row r="97" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>4</v>
       </c>
-      <c r="J97" s="55" t="s">
+      <c r="J97" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="K97" s="55"/>
-      <c r="L97" s="55"/>
-      <c r="M97" s="55"/>
+      <c r="K97" s="60"/>
+      <c r="L97" s="60"/>
+      <c r="M97" s="60"/>
       <c r="N97" t="s">
         <v>1</v>
       </c>
@@ -6260,12 +6328,12 @@
       <c r="B98">
         <v>10</v>
       </c>
-      <c r="J98" s="55" t="s">
+      <c r="J98" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="K98" s="55"/>
-      <c r="L98" s="55"/>
-      <c r="M98" s="55"/>
+      <c r="K98" s="60"/>
+      <c r="L98" s="60"/>
+      <c r="M98" s="60"/>
       <c r="N98">
         <v>2</v>
       </c>
@@ -6277,12 +6345,12 @@
       <c r="B99">
         <v>6</v>
       </c>
-      <c r="J99" s="55" t="s">
+      <c r="J99" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="K99" s="55"/>
-      <c r="L99" s="55"/>
-      <c r="M99" s="55"/>
+      <c r="K99" s="60"/>
+      <c r="L99" s="60"/>
+      <c r="M99" s="60"/>
       <c r="N99">
         <v>7</v>
       </c>
@@ -6318,14 +6386,14 @@
       </c>
     </row>
     <row r="104" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="N104" s="55" t="s">
+      <c r="N104" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="O104" s="55"/>
+      <c r="O104" s="60"/>
     </row>
     <row r="105" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="N105" s="55"/>
-      <c r="O105" s="55"/>
+      <c r="N105" s="60"/>
+      <c r="O105" s="60"/>
     </row>
     <row r="106" spans="2:15" x14ac:dyDescent="0.25">
       <c r="N106" t="s">
@@ -6373,31 +6441,31 @@
       </c>
     </row>
     <row r="122" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K122" s="54" t="s">
+      <c r="K122" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="L122" s="55"/>
+      <c r="L122" s="60"/>
     </row>
     <row r="123" spans="11:13" x14ac:dyDescent="0.25">
-      <c r="K123" s="55" t="s">
+      <c r="K123" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="L123" s="55"/>
+      <c r="L123" s="60"/>
       <c r="M123" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="135" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="55" t="s">
+      <c r="A135" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B135" s="55"/>
-      <c r="C135" s="55"/>
-      <c r="D135" s="55"/>
-      <c r="E135" s="55"/>
-      <c r="F135" s="55"/>
-      <c r="G135" s="55"/>
-      <c r="H135" s="55"/>
+      <c r="B135" s="60"/>
+      <c r="C135" s="60"/>
+      <c r="D135" s="60"/>
+      <c r="E135" s="60"/>
+      <c r="F135" s="60"/>
+      <c r="G135" s="60"/>
+      <c r="H135" s="60"/>
       <c r="J135" t="s">
         <v>64</v>
       </c>
@@ -6805,16 +6873,16 @@
       </c>
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A153" s="55" t="s">
+      <c r="A153" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="B153" s="55"/>
-      <c r="C153" s="55"/>
-      <c r="D153" s="55"/>
-      <c r="E153" s="55"/>
-      <c r="F153" s="55"/>
-      <c r="G153" s="55"/>
-      <c r="H153" s="55"/>
+      <c r="B153" s="60"/>
+      <c r="C153" s="60"/>
+      <c r="D153" s="60"/>
+      <c r="E153" s="60"/>
+      <c r="F153" s="60"/>
+      <c r="G153" s="60"/>
+      <c r="H153" s="60"/>
       <c r="I153" t="s">
         <v>82</v>
       </c>
@@ -6860,20 +6928,20 @@
       </c>
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J160" s="54" t="s">
+      <c r="J160" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="K160" s="55"/>
+      <c r="K160" s="60"/>
     </row>
     <row r="161" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J161" s="55" t="s">
+      <c r="J161" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K161" s="55"/>
-      <c r="L161" s="55"/>
-      <c r="M161" s="55"/>
-      <c r="N161" s="55"/>
-      <c r="O161" s="55"/>
+      <c r="K161" s="60"/>
+      <c r="L161" s="60"/>
+      <c r="M161" s="60"/>
+      <c r="N161" s="60"/>
+      <c r="O161" s="60"/>
     </row>
     <row r="162" spans="10:15" x14ac:dyDescent="0.25">
       <c r="J162" t="s">
@@ -6903,15 +6971,15 @@
       </c>
     </row>
     <row r="185" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J185" s="55" t="s">
+      <c r="J185" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="K185" s="55"/>
-      <c r="L185" s="55"/>
-      <c r="M185" s="55"/>
-      <c r="N185" s="55"/>
-      <c r="O185" s="55"/>
-      <c r="P185" s="55"/>
+      <c r="K185" s="60"/>
+      <c r="L185" s="60"/>
+      <c r="M185" s="60"/>
+      <c r="N185" s="60"/>
+      <c r="O185" s="60"/>
+      <c r="P185" s="60"/>
     </row>
     <row r="186" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="42" t="s">
@@ -7067,16 +7135,16 @@
       </c>
     </row>
     <row r="236" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A236" s="55" t="s">
+      <c r="A236" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="B236" s="55"/>
-      <c r="C236" s="55"/>
-      <c r="D236" s="55"/>
-      <c r="E236" s="55"/>
-      <c r="F236" s="55"/>
-      <c r="G236" s="55"/>
-      <c r="H236" s="55"/>
+      <c r="B236" s="60"/>
+      <c r="C236" s="60"/>
+      <c r="D236" s="60"/>
+      <c r="E236" s="60"/>
+      <c r="F236" s="60"/>
+      <c r="G236" s="60"/>
+      <c r="H236" s="60"/>
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
@@ -7476,10 +7544,10 @@
       </c>
     </row>
     <row r="290" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I290" s="54" t="s">
+      <c r="I290" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="J290" s="55"/>
+      <c r="J290" s="60"/>
     </row>
     <row r="291" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J291" t="s">
@@ -7499,10 +7567,10 @@
       <c r="C292" t="s">
         <v>103</v>
       </c>
-      <c r="I292" s="54" t="s">
+      <c r="I292" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="J292" s="55"/>
+      <c r="J292" s="60"/>
       <c r="M292" t="s">
         <v>121</v>
       </c>
@@ -7790,7 +7858,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="337" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B337" t="s">
         <v>1</v>
       </c>
@@ -7810,7 +7878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="338" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B338" t="s">
         <v>22</v>
       </c>
@@ -7829,8 +7897,51 @@
       <c r="G338">
         <v>5</v>
       </c>
-    </row>
-    <row r="342" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K338" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="339" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J339" t="s">
+        <v>65</v>
+      </c>
+      <c r="K339" s="53" t="s">
+        <v>141</v>
+      </c>
+      <c r="L339" t="s">
+        <v>142</v>
+      </c>
+      <c r="M339" t="s">
+        <v>143</v>
+      </c>
+      <c r="N339" t="s">
+        <v>144</v>
+      </c>
+      <c r="O339" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="340" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J340" t="s">
+        <v>102</v>
+      </c>
+      <c r="K340">
+        <v>2</v>
+      </c>
+      <c r="L340">
+        <v>10</v>
+      </c>
+      <c r="M340">
+        <v>20</v>
+      </c>
+      <c r="N340">
+        <v>6</v>
+      </c>
+      <c r="O340">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="342" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>1</v>
       </c>
@@ -7843,8 +7954,11 @@
       <c r="D342" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="343" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I342" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="343" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>0</v>
       </c>
@@ -7859,8 +7973,29 @@
         <f>B355*$B$348</f>
         <v>1.02581787109375</v>
       </c>
-    </row>
-    <row r="344" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J343" t="s">
+        <v>65</v>
+      </c>
+      <c r="K343" t="s">
+        <v>102</v>
+      </c>
+      <c r="L343" t="s">
+        <v>113</v>
+      </c>
+      <c r="M343" t="s">
+        <v>114</v>
+      </c>
+      <c r="N343" t="s">
+        <v>1</v>
+      </c>
+      <c r="O343" t="s">
+        <v>23</v>
+      </c>
+      <c r="P343" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="344" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>1</v>
       </c>
@@ -7875,8 +8010,33 @@
         <f t="shared" ref="D344:D347" si="15">B356*$B$348</f>
         <v>5.2756347656250009</v>
       </c>
-    </row>
-    <row r="345" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J344" t="s">
+        <v>141</v>
+      </c>
+      <c r="K344">
+        <v>2</v>
+      </c>
+      <c r="L344">
+        <v>10</v>
+      </c>
+      <c r="M344">
+        <f>L344+5</f>
+        <v>15</v>
+      </c>
+      <c r="N344">
+        <f>(M344+L344)/2</f>
+        <v>12.5</v>
+      </c>
+      <c r="O344">
+        <f>K344*N344</f>
+        <v>25</v>
+      </c>
+      <c r="P344">
+        <f>(N344*N344)*K344</f>
+        <v>312.5</v>
+      </c>
+    </row>
+    <row r="345" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>2</v>
       </c>
@@ -7891,8 +8051,33 @@
         <f t="shared" si="15"/>
         <v>10.174438476562502</v>
       </c>
-    </row>
-    <row r="346" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J345" t="s">
+        <v>142</v>
+      </c>
+      <c r="K345">
+        <v>10</v>
+      </c>
+      <c r="L345">
+        <v>15</v>
+      </c>
+      <c r="M345">
+        <f t="shared" ref="M345:M348" si="16">L345+5</f>
+        <v>20</v>
+      </c>
+      <c r="N345">
+        <f t="shared" ref="N345:N348" si="17">(M345+L345)/2</f>
+        <v>17.5</v>
+      </c>
+      <c r="O345">
+        <f t="shared" ref="O345:O348" si="18">K345*N345</f>
+        <v>175</v>
+      </c>
+      <c r="P345">
+        <f t="shared" ref="P345:P348" si="19">(N345*N345)*K345</f>
+        <v>3062.5</v>
+      </c>
+    </row>
+    <row r="346" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>3</v>
       </c>
@@ -7907,8 +8092,33 @@
         <f t="shared" si="15"/>
         <v>8.7209472656249982</v>
       </c>
-    </row>
-    <row r="347" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J346" t="s">
+        <v>143</v>
+      </c>
+      <c r="K346">
+        <v>20</v>
+      </c>
+      <c r="L346">
+        <v>20</v>
+      </c>
+      <c r="M346">
+        <f t="shared" si="16"/>
+        <v>25</v>
+      </c>
+      <c r="N346">
+        <f t="shared" si="17"/>
+        <v>22.5</v>
+      </c>
+      <c r="O346">
+        <f t="shared" si="18"/>
+        <v>450</v>
+      </c>
+      <c r="P346">
+        <f t="shared" si="19"/>
+        <v>10125</v>
+      </c>
+    </row>
+    <row r="347" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>4</v>
       </c>
@@ -7923,8 +8133,33 @@
         <f t="shared" si="15"/>
         <v>2.8031616210937509</v>
       </c>
-    </row>
-    <row r="348" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J347" t="s">
+        <v>144</v>
+      </c>
+      <c r="K347">
+        <v>6</v>
+      </c>
+      <c r="L347">
+        <v>25</v>
+      </c>
+      <c r="M347">
+        <f t="shared" si="16"/>
+        <v>30</v>
+      </c>
+      <c r="N347">
+        <f t="shared" si="17"/>
+        <v>27.5</v>
+      </c>
+      <c r="O347">
+        <f t="shared" si="18"/>
+        <v>165</v>
+      </c>
+      <c r="P347">
+        <f t="shared" si="19"/>
+        <v>4537.5</v>
+      </c>
+    </row>
+    <row r="348" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>51</v>
       </c>
@@ -7940,8 +8175,50 @@
         <f>SUM(D343:D347)</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="350" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J348" t="s">
+        <v>145</v>
+      </c>
+      <c r="K348">
+        <v>3</v>
+      </c>
+      <c r="L348">
+        <v>30</v>
+      </c>
+      <c r="M348">
+        <f t="shared" si="16"/>
+        <v>35</v>
+      </c>
+      <c r="N348">
+        <f t="shared" si="17"/>
+        <v>32.5</v>
+      </c>
+      <c r="O348">
+        <f t="shared" si="18"/>
+        <v>97.5</v>
+      </c>
+      <c r="P348">
+        <f t="shared" si="19"/>
+        <v>3168.75</v>
+      </c>
+    </row>
+    <row r="349" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J349" t="s">
+        <v>147</v>
+      </c>
+      <c r="K349">
+        <f>SUM(K344:K348)</f>
+        <v>41</v>
+      </c>
+      <c r="O349">
+        <f>SUM(O344:O348)</f>
+        <v>912.5</v>
+      </c>
+      <c r="P349">
+        <f>SUM(P344:P348)</f>
+        <v>21206.25</v>
+      </c>
+    </row>
+    <row r="350" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>77</v>
       </c>
@@ -7950,15 +8227,22 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="351" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>27</v>
       </c>
       <c r="B351">
         <v>2.25</v>
       </c>
-    </row>
-    <row r="352" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I351" t="s">
+        <v>77</v>
+      </c>
+      <c r="J351" s="11">
+        <f>O349/K349</f>
+        <v>22.256097560975611</v>
+      </c>
+    </row>
+    <row r="352" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>25</v>
       </c>
@@ -7966,6 +8250,13 @@
         <f>B351/4</f>
         <v>0.5625</v>
       </c>
+      <c r="I352" t="s">
+        <v>40</v>
+      </c>
+      <c r="J352" s="11">
+        <f>SQRT(1/K349*P349-(J351^2))</f>
+        <v>4.6788600227441126</v>
+      </c>
     </row>
     <row r="353" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
@@ -7990,7 +8281,7 @@
         <v>132</v>
       </c>
       <c r="B356">
-        <f t="shared" ref="B356:B359" si="16">_xlfn.BINOM.DIST(A344,4,$B$352,0)</f>
+        <f t="shared" ref="B356:B359" si="20">_xlfn.BINOM.DIST(A344,4,$B$352,0)</f>
         <v>0.18841552734375003</v>
       </c>
     </row>
@@ -7999,7 +8290,7 @@
         <v>133</v>
       </c>
       <c r="B357">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.36337280273437506</v>
       </c>
     </row>
@@ -8008,7 +8299,7 @@
         <v>134</v>
       </c>
       <c r="B358">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.31146240234374994</v>
       </c>
     </row>
@@ -8017,7 +8308,7 @@
         <v>135</v>
       </c>
       <c r="B359">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.10011291503906253</v>
       </c>
     </row>
@@ -8041,47 +8332,236 @@
       </c>
     </row>
     <row r="364" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A364" s="61" t="s">
+      <c r="A364" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B364" s="62">
+      <c r="B364" s="55">
         <v>0</v>
       </c>
-      <c r="C364" s="62">
+      <c r="C364" s="55">
         <v>1</v>
       </c>
-      <c r="D364" s="62">
+      <c r="D364" s="55">
         <v>2</v>
       </c>
-      <c r="E364" s="62">
+      <c r="E364" s="55">
         <v>3</v>
       </c>
-      <c r="F364" s="63">
+      <c r="F364" s="56">
         <v>4</v>
       </c>
     </row>
     <row r="365" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A365" s="64" t="s">
+      <c r="A365" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="B365" s="65">
+      <c r="B365" s="58">
         <v>1.02581787109375</v>
       </c>
-      <c r="C365" s="65">
+      <c r="C365" s="58">
         <v>5.2756347656250009</v>
       </c>
-      <c r="D365" s="65">
+      <c r="D365" s="58">
         <v>10.174438476562502</v>
       </c>
-      <c r="E365" s="65">
+      <c r="E365" s="58">
         <v>8.7209472656249982</v>
       </c>
-      <c r="F365" s="66">
+      <c r="F365" s="59">
         <v>2.8031616210937509</v>
+      </c>
+    </row>
+    <row r="386" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I386" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="387" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B387" t="s">
+        <v>148</v>
+      </c>
+      <c r="I387" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="388" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B388" t="s">
+        <v>149</v>
+      </c>
+      <c r="I388" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="389" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>51</v>
+      </c>
+      <c r="B389">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="390" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A390" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B390">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="391" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A391" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B391">
+        <v>1.5</v>
+      </c>
+      <c r="I391" t="s">
+        <v>51</v>
+      </c>
+      <c r="J391">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="392" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A392" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B392">
+        <v>0.05</v>
+      </c>
+      <c r="C392" t="s">
+        <v>151</v>
+      </c>
+      <c r="D392">
+        <f>1-B392/2</f>
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="I392" t="s">
+        <v>161</v>
+      </c>
+      <c r="J392">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="393" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>150</v>
+      </c>
+      <c r="B393" s="67">
+        <f>_xlfn.NORM.S.INV(D392)</f>
+        <v>1.9599639845400536</v>
+      </c>
+      <c r="I393" t="s">
+        <v>40</v>
+      </c>
+      <c r="J393">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="394" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>153</v>
+      </c>
+      <c r="B394" s="51">
+        <f>B391/SQRT(B389)</f>
+        <v>0.21213203435596426</v>
+      </c>
+      <c r="I394" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="J394">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="395" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>52</v>
+      </c>
+      <c r="B395" s="51">
+        <f>B393*B394</f>
+        <v>0.41577114730490322</v>
+      </c>
+      <c r="I395" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J395">
+        <f>J392-J394</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="396" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A396" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B396" s="67">
+        <f>B390-B395</f>
+        <v>74.584228852695091</v>
+      </c>
+      <c r="I396" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J396">
+        <f>J393/SQRT(J391)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="397" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A397" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B397" s="67">
+        <f>B390+B395</f>
+        <v>75.415771147304909</v>
+      </c>
+      <c r="I397" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J397">
+        <f>J395/J396</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="398" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I398" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J398">
+        <f>_xlfn.NORM.S.INV(0.975)</f>
+        <v>1.9599639845400536</v>
+      </c>
+    </row>
+    <row r="400" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I400" t="str">
+        <f>IF(J397&lt;J398,"Null Hypothesis is accepted","Null Hypothesis is rejected")</f>
+        <v>Null Hypothesis is rejected</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="I290:J290"/>
+    <mergeCell ref="I292:J292"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="J98:M98"/>
+    <mergeCell ref="J99:M99"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:N17"/>
+    <mergeCell ref="K12:N13"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:N15"/>
+    <mergeCell ref="K48:L49"/>
+    <mergeCell ref="K88:O89"/>
+    <mergeCell ref="K93:P93"/>
+    <mergeCell ref="J96:K96"/>
+    <mergeCell ref="J97:M97"/>
+    <mergeCell ref="N96:O96"/>
     <mergeCell ref="N104:O105"/>
     <mergeCell ref="K122:L122"/>
     <mergeCell ref="K123:L123"/>
@@ -8091,30 +8571,6 @@
     <mergeCell ref="J160:K160"/>
     <mergeCell ref="J161:O161"/>
     <mergeCell ref="J185:P185"/>
-    <mergeCell ref="K48:L49"/>
-    <mergeCell ref="K88:O89"/>
-    <mergeCell ref="K93:P93"/>
-    <mergeCell ref="J96:K96"/>
-    <mergeCell ref="J97:M97"/>
-    <mergeCell ref="N96:O96"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L16:N17"/>
-    <mergeCell ref="K12:N13"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:N15"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="I290:J290"/>
-    <mergeCell ref="I292:J292"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="J98:M98"/>
-    <mergeCell ref="J99:M99"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>